<commit_message>
chore: add @adobe/aio-cli-plugin-app to health.xlsx
</commit_message>
<xml_diff>
--- a/health.xlsx
+++ b/health.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shazron/Documents/git/adobe/aio-cli/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaz/git/adobe/aio-cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945270E5-1F76-7C43-BC92-A6133112BE05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033E05A2-1F32-894F-BC1A-C41E88417302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="460" windowWidth="25580" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3520" yWindow="460" windowWidth="25580" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Module</t>
   </si>
@@ -146,6 +146,27 @@
   </si>
   <si>
     <t>[![Github Pull Requests](https://img.shields.io/github/issues-pr/adobe/aio-cli-plugin-jwt-auth.svg)](https://github.com/adobe/aio-cli-plugin-jwt-auth/pulls)</t>
+  </si>
+  <si>
+    <t>@adobe/aio-cli-plugin-app</t>
+  </si>
+  <si>
+    <t>[![Version](https://img.shields.io/npm/v/@adobe/aio-cli-plugin-app.svg)](https://npmjs.org/package/@adobe/aio-cli-plugin-app)</t>
+  </si>
+  <si>
+    <t>[![Downloads/week](https://img.shields.io/npm/dw/@adobe/aio-cli-plugin-app.svg)](https://npmjs.org/package/@adobe/aio-cli-plugin-app)</t>
+  </si>
+  <si>
+    <t>[![Build Status](https://travis-ci.com/adobe/aio-cli-plugin-app.svg?branch=master)](https://travis-ci.com/adobe/aio-cli-plugin-app)</t>
+  </si>
+  <si>
+    <t>[![Codecov Coverage](https://img.shields.io/codecov/c/github/adobe/aio-cli-plugin-app/master.svg?style=flat-square)](https://codecov.io/gh/adobe/aio-cli-plugin-app/)</t>
+  </si>
+  <si>
+    <t>[![Github Issues](https://img.shields.io/github/issues/adobe/aio-cli-plugin-app.svg)](https://github.com/adobe/aio-cli-plugin-app/issues)</t>
+  </si>
+  <si>
+    <t>[![Github Pull Requests](https://img.shields.io/github/issues-pr/adobe/aio-cli-plugin-app.svg)](https://github.com/adobe/aio-cli-plugin-app/pulls)</t>
   </si>
 </sst>
 </file>
@@ -440,7 +461,7 @@
   <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection sqref="A1:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -587,13 +608,27 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7"/>

</xml_diff>

<commit_message>
Add @adobe/aio-cli-plugin-auth to health table
</commit_message>
<xml_diff>
--- a/health.xlsx
+++ b/health.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shazron/Documents/git/adobe/aio-cli/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaz/git/adobe/aio-cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC56971F-C495-F44C-81BB-482A92F1E1F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D406036-C57F-D94C-8168-89C82BF047A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="460" windowWidth="25580" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3520" yWindow="460" windowWidth="39840" windowHeight="25400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Module</t>
   </si>
@@ -196,6 +196,27 @@
   </si>
   <si>
     <t>@adobe/aio-cli-plugin-ims</t>
+  </si>
+  <si>
+    <t>@adobe/aio-cli-plugin-auth</t>
+  </si>
+  <si>
+    <t>[![Version](https://img.shields.io/npm/v/@adobe/aio-cli-plugin-auth.svg)](https://npmjs.org/package/@adobe/aio-cli-plugin-auth)</t>
+  </si>
+  <si>
+    <t>[![Downloads/week](https://img.shields.io/npm/dw/@adobe/aio-cli-plugin-auth.svg)](https://npmjs.org/package/@adobe/aio-cli-plugin-auth)</t>
+  </si>
+  <si>
+    <t>[![Build Status](https://travis-ci.com/adobe/aio-cli-plugin-auth.svg?branch=master)](https://travis-ci.com/adobe/aio-cli-plugin-auth)</t>
+  </si>
+  <si>
+    <t>[![Codecov Coverage](https://img.shields.io/codecov/c/github/adobe/aio-cli-plugin-auth/master.svg?style=flat-square)](https://codecov.io/gh/adobe/aio-cli-plugin-auth/)</t>
+  </si>
+  <si>
+    <t>[![Github Issues](https://img.shields.io/github/issues/adobe/aio-cli-plugin-auth.svg)](https://github.com/adobe/aio-cli-plugin-auth/issues)</t>
+  </si>
+  <si>
+    <t>[![Github Pull Requests](https://img.shields.io/github/issues-pr/adobe/aio-cli-plugin-auth.svg)](https://github.com/adobe/aio-cli-plugin-auth/pulls)</t>
   </si>
 </sst>
 </file>
@@ -490,7 +511,7 @@
   <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -684,13 +705,27 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="A9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>

</xml_diff>